<commit_message>
added multi batch compatibility
</commit_message>
<xml_diff>
--- a/student_codes.xlsx
+++ b/student_codes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -70,18 +70,6 @@
     <t xml:space="preserve">bilalmohussain24@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Camelia Ignat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/avocami</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cignat70@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Daniel Biman</t>
   </si>
   <si>
@@ -200,18 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">madina1110000@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magdalena Mostazo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/magdalenammcc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">magdalenammcc@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Mark Skinner</t>
@@ -711,10 +687,10 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="1" sqref="D48 E38"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="A18:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43"/>
@@ -784,157 +760,149 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="A6" s="11"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,199 +912,191 @@
       <c r="D17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="A18" s="11"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1144,31 +1104,29 @@
     <hyperlink ref="C2" r:id="rId1" display="https://github.com/AgathiyaRaja"/>
     <hyperlink ref="C3" r:id="rId2" display="https://github.com/alessiorecchia"/>
     <hyperlink ref="C5" r:id="rId3" display="https://github.com/bills24"/>
-    <hyperlink ref="C6" r:id="rId4" display="https://github.com/avocami"/>
-    <hyperlink ref="C7" r:id="rId5" display="https://github.com/DanielBiman"/>
-    <hyperlink ref="C8" r:id="rId6" display="https://github.com/Deniz-shelby"/>
-    <hyperlink ref="C9" r:id="rId7" display="https://github.com/fistadev"/>
-    <hyperlink ref="C10" r:id="rId8" display="https://github.com/fbulbulov/"/>
-    <hyperlink ref="C11" r:id="rId9" display="https://github.com/Calypso25"/>
-    <hyperlink ref="C12" r:id="rId10" display="https://github.com/Gawasinspire"/>
-    <hyperlink ref="C13" r:id="rId11" display="https://github.com/HedayaAli"/>
-    <hyperlink ref="C14" r:id="rId12" display="https://github.com/Josh-Batt"/>
-    <hyperlink ref="C15" r:id="rId13" display="https://github.com/Pathi-rao"/>
-    <hyperlink ref="C16" r:id="rId14" display="https://github.com/madinach"/>
-    <hyperlink ref="C18" r:id="rId15" display="https://github.com/magdalenammcc"/>
-    <hyperlink ref="C19" r:id="rId16" display="https://github.com/aimwps"/>
-    <hyperlink ref="C20" r:id="rId17" display="https://github.com/M-C-AD"/>
-    <hyperlink ref="C21" r:id="rId18" display="https://github.com/nsarkhanov"/>
-    <hyperlink ref="C22" r:id="rId19" display="https://github.com/salamituns"/>
-    <hyperlink ref="C23" r:id="rId20" display="https://github.com/Marzipan78"/>
-    <hyperlink ref="C24" r:id="rId21" display="https://github.com/zoeynguyen1719"/>
-    <hyperlink ref="C25" r:id="rId22" display="https://github.com/shahidqureshi01"/>
-    <hyperlink ref="C26" r:id="rId23" display="https://github.com/stephengeorge93"/>
-    <hyperlink ref="C27" r:id="rId24" display="https://github.com/Sven-Skyth-Henriksen"/>
-    <hyperlink ref="C28" r:id="rId25" display="https://github.com/Tomjohnsonellis"/>
-    <hyperlink ref="C29" r:id="rId26" display="https://github.com/UdawalaHewageDilan"/>
-    <hyperlink ref="C30" r:id="rId27" display="https://github.com/aktumut"/>
-    <hyperlink ref="C31" r:id="rId28" display="https://github.com/VladimirGas"/>
+    <hyperlink ref="C7" r:id="rId4" display="https://github.com/DanielBiman"/>
+    <hyperlink ref="C8" r:id="rId5" display="https://github.com/Deniz-shelby"/>
+    <hyperlink ref="C9" r:id="rId6" display="https://github.com/fistadev"/>
+    <hyperlink ref="C10" r:id="rId7" display="https://github.com/fbulbulov/"/>
+    <hyperlink ref="C11" r:id="rId8" display="https://github.com/Calypso25"/>
+    <hyperlink ref="C12" r:id="rId9" display="https://github.com/Gawasinspire"/>
+    <hyperlink ref="C13" r:id="rId10" display="https://github.com/HedayaAli"/>
+    <hyperlink ref="C14" r:id="rId11" display="https://github.com/Josh-Batt"/>
+    <hyperlink ref="C15" r:id="rId12" display="https://github.com/Pathi-rao"/>
+    <hyperlink ref="C16" r:id="rId13" display="https://github.com/madinach"/>
+    <hyperlink ref="C19" r:id="rId14" display="https://github.com/aimwps"/>
+    <hyperlink ref="C20" r:id="rId15" display="https://github.com/M-C-AD"/>
+    <hyperlink ref="C21" r:id="rId16" display="https://github.com/nsarkhanov"/>
+    <hyperlink ref="C22" r:id="rId17" display="https://github.com/salamituns"/>
+    <hyperlink ref="C23" r:id="rId18" display="https://github.com/Marzipan78"/>
+    <hyperlink ref="C24" r:id="rId19" display="https://github.com/zoeynguyen1719"/>
+    <hyperlink ref="C25" r:id="rId20" display="https://github.com/shahidqureshi01"/>
+    <hyperlink ref="C26" r:id="rId21" display="https://github.com/stephengeorge93"/>
+    <hyperlink ref="C27" r:id="rId22" display="https://github.com/Sven-Skyth-Henriksen"/>
+    <hyperlink ref="C28" r:id="rId23" display="https://github.com/Tomjohnsonellis"/>
+    <hyperlink ref="C29" r:id="rId24" display="https://github.com/UdawalaHewageDilan"/>
+    <hyperlink ref="C30" r:id="rId25" display="https://github.com/aktumut"/>
+    <hyperlink ref="C31" r:id="rId26" display="https://github.com/VladimirGas"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>